<commit_message>
intial working code reading from excel
</commit_message>
<xml_diff>
--- a/CuccumberFromExcel/src/main/resources/test.xlsx
+++ b/CuccumberFromExcel/src/main/resources/test.xlsx
@@ -15,12 +15,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>visgag</t>
   </si>
   <si>
-    <t>test</t>
+    <t>Tester went to bank to deposit money</t>
+  </si>
+  <si>
+    <t>bank</t>
+  </si>
+  <si>
+    <t>Tester went to banks of river for fishing</t>
+  </si>
+  <si>
+    <t>I went fishing for some sea bass.</t>
+  </si>
+  <si>
+    <t>The bass line of the song is too weak.</t>
+  </si>
+  <si>
+    <t>bass</t>
   </si>
 </sst>
 </file>
@@ -380,18 +395,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>